<commit_message>
Bugfix initial database import
</commit_message>
<xml_diff>
--- a/NamingConventionTool/src/main/java/org/openepics/names/services/NamingDatabaseImport.xlsx
+++ b/NamingConventionTool/src/main/java/org/openepics/names/services/NamingDatabaseImport.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31040" windowHeight="15600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="AreaStructure" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DeviceStructure" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="DeviceInstances" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="AreaStructure" sheetId="1" r:id="rId1"/>
+    <sheet name="DeviceStructure" sheetId="2" r:id="rId2"/>
+    <sheet name="DeviceInstances" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -121,48 +125,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <color rgb="FFA6A6A6"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FFA6A6A6"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,7 +159,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -182,61 +167,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -295,33 +246,354 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E8" activeCellId="0" pane="topLeft" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0056179775281"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4325842696629"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8483146067416"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.185393258427"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="21.8483146067416"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" spans="1:1024">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -338,25 +610,25 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2" s="4">
+    <row r="2" spans="1:1024" s="4" customFormat="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>10001</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="2" t="n">
+      <c r="AMJ2"/>
+    </row>
+    <row r="3" spans="1:1024">
+      <c r="A3" s="2">
         <v>10001</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="2">
         <v>11001</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -365,15 +637,15 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:1024">
+      <c r="A4" s="2">
         <v>11001</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>12001</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -382,60 +654,53 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:1024">
+      <c r="A5">
         <v>12001</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>13001</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E2" activeCellId="0" pane="topLeft" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD475"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0056179775281"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4325842696629"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8483146067416"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.4269662921348"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="21.8483146067416"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" spans="1:1024">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,26 +717,26 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2" s="4">
+    <row r="2" spans="1:1024" s="4" customFormat="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>20001</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="2" t="n">
+      <c r="AMI2"/>
+      <c r="AMJ2"/>
+    </row>
+    <row r="3" spans="1:1024">
+      <c r="A3" s="2">
         <v>20001</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="2">
         <v>21001</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -480,15 +745,15 @@
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:1024">
+      <c r="A4" s="2">
         <v>21001</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>22001</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -497,55 +762,55 @@
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:1024">
+      <c r="A5">
         <v>22001</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>23001</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="21.8483146067416"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -562,30 +827,30 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="n">
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="2">
         <v>13001</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>23001</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>